<commit_message>
Latex Verslag toegevoegd + Gantt klaar
</commit_message>
<xml_diff>
--- a/Gantt Chart 05102015.xlsx
+++ b/Gantt Chart 05102015.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="PercentageVoltooid">PercentageVoltooidNa*PeriodeInPlan</definedName>
     <definedName name="PercentageVoltooidNa">(project!A$8=MEDIAN(project!A$8,project!$E1,project!$E1+project!$F1)*(project!$E1&gt;0))*((project!A$8&lt;(INT(project!$E1+project!$F1*project!$G1)))+(project!A$8=project!$E1))*(project!$G1&gt;0)</definedName>
-    <definedName name="periode_geselecteerd">project!$P$3</definedName>
+    <definedName name="periode_geselecteerd">project!$M$3</definedName>
     <definedName name="PeriodeInPlan">project!A$8=MEDIAN(project!A$8,project!$C1,project!$C1+project!$D1-1)</definedName>
     <definedName name="PeriodeInWerkelijk">project!A$8=MEDIAN(project!A$8,project!$E1,project!$E1+project!$F1-1)</definedName>
     <definedName name="Plan">PeriodeInPlan*(project!$C1&gt;0)</definedName>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="81">
   <si>
     <t>Plan</t>
   </si>
@@ -299,6 +299,33 @@
   </si>
   <si>
     <t>Final report</t>
+  </si>
+  <si>
+    <t>Frederik, Arne, Kristof</t>
+  </si>
+  <si>
+    <t>Kristof, Arno</t>
+  </si>
+  <si>
+    <t>Arne, Wouter, Pieter</t>
+  </si>
+  <si>
+    <t>Arno, Kristof, Frederik</t>
+  </si>
+  <si>
+    <t>Kristof, Frederik, Pieter</t>
+  </si>
+  <si>
+    <t>Arne, Frederik, Arno</t>
+  </si>
+  <si>
+    <t>Arne, Frederik, Kristof</t>
+  </si>
+  <si>
+    <t>Frederik, Pieter, Wouter</t>
+  </si>
+  <si>
+    <t>Arno, Arne, Wouter</t>
   </si>
 </sst>
 </file>
@@ -816,13 +843,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>16</xdr:col>
+          <xdr:col>13</xdr:col>
           <xdr:colOff>66675</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>16</xdr:col>
+          <xdr:col>13</xdr:col>
           <xdr:colOff>200025</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>257175</xdr:rowOff>
@@ -1094,8 +1121,8 @@
   </sheetPr>
   <dimension ref="A2:BS36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1113,7 +1140,7 @@
     <col min="23" max="30" width="2.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:71" ht="54" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:71" ht="32.25" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B2" s="32" t="s">
         <v>11</v>
       </c>
@@ -1138,36 +1165,32 @@
         <v>8</v>
       </c>
       <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="19">
+      <c r="M3" s="19">
         <v>2</v>
       </c>
-      <c r="Q3" s="8"/>
-      <c r="S3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="10"/>
       <c r="T3" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="V3" s="10"/>
-      <c r="W3" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="6" t="s">
+      <c r="U3" s="11"/>
+      <c r="V3" s="6" t="s">
         <v>59</v>
       </c>
+      <c r="Z3" s="12"/>
+      <c r="AA3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB3"/>
+      <c r="AC3"/>
       <c r="AE3" s="1"/>
-      <c r="AF3" s="12"/>
-      <c r="AG3" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1"/>
-      <c r="AM3" s="1"/>
-      <c r="AQ3" s="13"/>
-      <c r="AR3" s="6" t="s">
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AK3" s="13"/>
+      <c r="AL3" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1409,7 +1432,7 @@
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="16">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H10" s="30" t="s">
         <v>63</v>
@@ -1776,7 +1799,9 @@
       <c r="H19" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="I19" s="16"/>
+      <c r="I19" s="16" t="s">
+        <v>72</v>
+      </c>
       <c r="P19" s="22"/>
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
@@ -1813,7 +1838,9 @@
       <c r="H20" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="I20" s="16"/>
+      <c r="I20" s="16" t="s">
+        <v>73</v>
+      </c>
       <c r="P20" s="22"/>
       <c r="AE20" s="1"/>
       <c r="AF20" s="1"/>
@@ -1850,7 +1877,9 @@
       <c r="H21" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="I21" s="16"/>
+      <c r="I21" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="P21" s="22"/>
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
@@ -1921,7 +1950,9 @@
       <c r="D23" s="15">
         <v>3</v>
       </c>
-      <c r="E23" s="15"/>
+      <c r="E23" s="15">
+        <v>2</v>
+      </c>
       <c r="F23" s="15"/>
       <c r="G23" s="16">
         <v>0</v>
@@ -2007,7 +2038,9 @@
       <c r="H25" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="I25" s="16"/>
+      <c r="I25" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="P25" s="22"/>
       <c r="AE25" s="1"/>
       <c r="AF25" s="1"/>
@@ -2044,7 +2077,9 @@
       <c r="H26" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="I26" s="16"/>
+      <c r="I26" s="16" t="s">
+        <v>75</v>
+      </c>
       <c r="P26" s="22"/>
       <c r="AE26" s="1"/>
       <c r="AF26" s="1"/>
@@ -2081,7 +2116,9 @@
       <c r="H27" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="I27" s="16"/>
+      <c r="I27" s="16" t="s">
+        <v>76</v>
+      </c>
       <c r="P27" s="22"/>
       <c r="AE27" s="1"/>
       <c r="AF27" s="1"/>
@@ -2118,7 +2155,9 @@
       <c r="H28" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="I28" s="16"/>
+      <c r="I28" s="16" t="s">
+        <v>77</v>
+      </c>
       <c r="P28" s="22"/>
       <c r="AE28" s="1"/>
       <c r="AF28" s="1"/>
@@ -2155,7 +2194,9 @@
       <c r="H29" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="I29" s="16"/>
+      <c r="I29" s="16" t="s">
+        <v>78</v>
+      </c>
       <c r="P29" s="22"/>
       <c r="AE29" s="1"/>
       <c r="AF29" s="1"/>
@@ -2192,7 +2233,9 @@
       <c r="H30" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="I30" s="16"/>
+      <c r="I30" s="16" t="s">
+        <v>79</v>
+      </c>
       <c r="P30" s="22"/>
       <c r="AE30" s="1"/>
       <c r="AF30" s="1"/>
@@ -2229,7 +2272,9 @@
       <c r="H31" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="I31" s="16"/>
+      <c r="I31" s="16" t="s">
+        <v>80</v>
+      </c>
       <c r="P31" s="22"/>
       <c r="AE31" s="1"/>
       <c r="AF31" s="1"/>
@@ -2465,13 +2510,13 @@
               <controlPr defaultSize="0" print="0" autoPict="0" altText="Period Highlight Spin Control">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>16</xdr:col>
+                    <xdr:col>13</xdr:col>
                     <xdr:colOff>66675</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>16</xdr:col>
+                    <xdr:col>13</xdr:col>
                     <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>257175</xdr:rowOff>

</xml_diff>